<commit_message>
Mest gjort tabeller och nya figurer i skripten för AIC-analyser. Har inte gjort något i skriptet för matade lyor. I boxplots ripdata har jag även gjort lite signifikanstester och figurer. I distance-samplingskripten har jag printat excelfiler för att göra tabeller i markdown. Även gjort en excelfil för kartdatat som jag importerat i markdown.
</commit_message>
<xml_diff>
--- a/GIS-data/tabell kartnamn i GIS-analysen.xlsx
+++ b/GIS-data/tabell kartnamn i GIS-analysen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/torhanssonfrank/Desktop/Skolarbeten/Master i Stockholm/Masterarbete/Den and territory selection/GIS-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A97E5E7-9F28-4A47-8A4D-B20EC57BEE31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15005E46-0F15-814A-B215-7236FA913934}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7420" yWindow="1440" windowWidth="24940" windowHeight="14140" xr2:uid="{E4ECEE93-8473-774A-BDDA-BF9BAD63ECCC}"/>
+    <workbookView xWindow="900" yWindow="3600" windowWidth="24940" windowHeight="14020" xr2:uid="{E4ECEE93-8473-774A-BDDA-BF9BAD63ECCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -135,7 +135,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -157,16 +157,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -174,55 +188,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -233,20 +235,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6CFA4292-9563-9A4C-89A5-CDABD3FA1152}" name="Tabell1" displayName="Tabell1" ref="B1:F8" totalsRowShown="0">
-  <autoFilter ref="B1:F8" xr:uid="{FC187B13-C294-3C48-8E52-8207C06EA7E9}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{3731EBDC-160D-0749-83A8-56B2A2747479}" name="Parameter"/>
-    <tableColumn id="2" xr3:uid="{D51595A1-29C6-124E-ABD7-0FCA5361091E}" name="Map" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{27A4A23A-A130-5D45-99F0-6B16ECAC7CCA}" name="Source"/>
-    <tableColumn id="4" xr3:uid="{91E73156-A2E7-F245-A662-A4C644818731}" name="Date downloaded" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{61179D24-2E69-0548-A683-54D05463A455}" name="Radius around den (m)"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -546,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2B54C7-7145-8448-BFC5-8DED97C7C4F3}">
-  <dimension ref="B1:F8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -559,131 +547,133 @@
     <col min="6" max="6" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F5">
+      <c r="E5" s="3">
         <v>1500</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="D6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F6">
+      <c r="E6" s="2">
         <v>1500</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F7">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3">
         <v>2500</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F8">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4">
         <v>1500</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>